<commit_message>
feat: adding some checks
</commit_message>
<xml_diff>
--- a/cluster_4.xlsx
+++ b/cluster_4.xlsx
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1362,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="AA11">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -2109,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="AA20">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -2192,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="AA21">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -2524,7 +2524,7 @@
         <v>1</v>
       </c>
       <c r="AA25">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -3022,7 +3022,7 @@
         <v>1</v>
       </c>
       <c r="AA31">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="AA34">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:27">
@@ -3354,7 +3354,7 @@
         <v>1</v>
       </c>
       <c r="AA35">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:27">
@@ -3520,7 +3520,7 @@
         <v>1</v>
       </c>
       <c r="AA37">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:27">
@@ -3686,7 +3686,7 @@
         <v>2</v>
       </c>
       <c r="AA39">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:27">
@@ -4018,7 +4018,7 @@
         <v>0</v>
       </c>
       <c r="AA43">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:27">
@@ -4848,7 +4848,7 @@
         <v>1</v>
       </c>
       <c r="AA53">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:27">
@@ -5014,7 +5014,7 @@
         <v>1</v>
       </c>
       <c r="AA55">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:27">
@@ -5927,7 +5927,7 @@
         <v>1</v>
       </c>
       <c r="AA66">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:27">
@@ -6425,7 +6425,7 @@
         <v>2</v>
       </c>
       <c r="AA72">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:27">
@@ -6840,7 +6840,7 @@
         <v>1</v>
       </c>
       <c r="AA77">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:27">
@@ -6923,7 +6923,7 @@
         <v>2</v>
       </c>
       <c r="AA78">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:27">
@@ -7504,7 +7504,7 @@
         <v>0</v>
       </c>
       <c r="AA85">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:27">
@@ -8002,7 +8002,7 @@
         <v>1</v>
       </c>
       <c r="AA91">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:27">
@@ -8085,7 +8085,7 @@
         <v>1</v>
       </c>
       <c r="AA92">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:27">
@@ -8417,7 +8417,7 @@
         <v>1</v>
       </c>
       <c r="AA96">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:27">
@@ -8749,7 +8749,7 @@
         <v>2</v>
       </c>
       <c r="AA100">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:27">
@@ -9413,7 +9413,7 @@
         <v>1</v>
       </c>
       <c r="AA108">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:27">
@@ -9745,7 +9745,7 @@
         <v>0</v>
       </c>
       <c r="AA112">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:27">
@@ -10492,7 +10492,7 @@
         <v>1</v>
       </c>
       <c r="AA121">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:27">
@@ -10575,7 +10575,7 @@
         <v>0</v>
       </c>
       <c r="AA122">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:27">
@@ -10824,7 +10824,7 @@
         <v>2</v>
       </c>
       <c r="AA125">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:27">
@@ -10990,7 +10990,7 @@
         <v>0</v>
       </c>
       <c r="AA127">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:27">
@@ -11156,7 +11156,7 @@
         <v>1</v>
       </c>
       <c r="AA129">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:27">
@@ -11322,7 +11322,7 @@
         <v>1</v>
       </c>
       <c r="AA131">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:27">
@@ -11488,7 +11488,7 @@
         <v>1</v>
       </c>
       <c r="AA133">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:27">
@@ -11820,7 +11820,7 @@
         <v>1</v>
       </c>
       <c r="AA137">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:27">
@@ -12318,7 +12318,7 @@
         <v>1</v>
       </c>
       <c r="AA143">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:27">
@@ -12401,7 +12401,7 @@
         <v>1</v>
       </c>
       <c r="AA144">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:27">
@@ -12484,7 +12484,7 @@
         <v>2</v>
       </c>
       <c r="AA145">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:27">
@@ -12733,7 +12733,7 @@
         <v>2</v>
       </c>
       <c r="AA148">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:27">
@@ -13231,7 +13231,7 @@
         <v>0</v>
       </c>
       <c r="AA154">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:27">
@@ -13314,7 +13314,7 @@
         <v>0</v>
       </c>
       <c r="AA155">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:27">
@@ -13480,7 +13480,7 @@
         <v>0</v>
       </c>
       <c r="AA157">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:27">
@@ -13563,7 +13563,7 @@
         <v>1</v>
       </c>
       <c r="AA158">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:27">

</xml_diff>